<commit_message>
fill empty in  0-50
</commit_message>
<xml_diff>
--- a/splited_sound_with_noise/splited_sound_with_noisesplited_sound_with_noise.xlsx
+++ b/splited_sound_with_noise/splited_sound_with_noisesplited_sound_with_noise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0 project\megacom\speech\splited_sound_with_noise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE80C5C-9F8B-4A49-AEFA-9C87BC1527F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E2BAAC-ED78-47D8-B7F6-71625EAFEFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="1895">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="1899">
   <si>
     <t>audio</t>
   </si>
@@ -5718,16 +5718,36 @@
   </si>
   <si>
     <t>بله خیلی ممنون  دست شما درد نکنه خواهش میکنم سلامت باشید خدانگهدار خدافظ خدافظ</t>
+  </si>
+  <si>
+    <t>جناب بار ارسالیم دارین  من شماره پلاک سی و دو هستم  صابعی</t>
+  </si>
+  <si>
+    <t>خانم زرندی  باش در خ از  خیلی مچکرم   قربان شما   خداحافظ  یا علی</t>
+  </si>
+  <si>
+    <t>* چند کیلوه هر کدوم از وز وزن ماهی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حالا باید بگیم </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5796,31 +5816,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
-    <cellStyle name="20% - Accent2" xfId="2" builtinId="34"/>
-    <cellStyle name="20% - Accent3" xfId="3" builtinId="38"/>
-    <cellStyle name="20% - Accent5" xfId="4" builtinId="46"/>
+  <cellStyles count="6">
+    <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
+    <cellStyle name="20% - Accent3" xfId="4" builtinId="38"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6123,8 +6146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1843"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6294,7 +6317,7 @@
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="6" t="str">
+      <c r="B14" s="7" t="str">
         <f>HYPERLINK("1739962654_15_SPK_0_20250215_v2.1739599940.2256629.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
@@ -6411,7 +6434,7 @@
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="6" t="str">
+      <c r="B24" s="7" t="str">
         <f>HYPERLINK("1739961628_0_SPK_0_20250213_v2.1739437852.2203015.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
@@ -6517,6 +6540,9 @@
         <f>HYPERLINK("1739961698_1_SPK_1_20250213_v2.1739437852.2203015.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C33" s="1" t="s">
+        <v>1897</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
@@ -6546,9 +6572,12 @@
       <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="6" t="str">
+      <c r="B36" s="7" t="str">
         <f>HYPERLINK("1739962606_5_SPK_0_20250215_v2.1739630799.2283007.wav", "Play Audio")</f>
         <v>Play Audio</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>1895</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -6559,6 +6588,9 @@
         <f>HYPERLINK("1739962360_8_SPK_0_20250216_v2.1739716378.2337553.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C37" s="1" t="s">
+        <v>1896</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
@@ -6612,12 +6644,12 @@
       <c r="A42" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="6" t="str">
+      <c r="B42" s="7" t="str">
         <f>HYPERLINK("1739962416_1_SPK_1_20250216_v2.1739698726.2310851.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1855</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fill 1-50 was empty
</commit_message>
<xml_diff>
--- a/splited_sound_with_noise/splited_sound_with_noisesplited_sound_with_noise.xlsx
+++ b/splited_sound_with_noise/splited_sound_with_noisesplited_sound_with_noise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0 project\megacom\speech\splited_sound_with_noise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E2BAAC-ED78-47D8-B7F6-71625EAFEFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FA40BB-EC24-4367-8BC0-B070F087F0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="105" yWindow="1575" windowWidth="13335" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="1899">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="1905">
   <si>
     <t>audio</t>
   </si>
@@ -5663,9 +5663,6 @@
     <t>ها قلوه گاه که کلا اصن به عنوان چربی استفاده میشه چون سینه  بوقلمونو رون بوقلمون خشکهه</t>
   </si>
   <si>
-    <t>عهه یه سوال داشتم از خدمتتون شما گوشت های چرخ کرده تون رو میشوریین یا نه</t>
-  </si>
-  <si>
     <t>واستا الان  میام میام چشم چشم قربونت  کیلو چنده مرغ</t>
   </si>
   <si>
@@ -5729,7 +5726,28 @@
     <t>* چند کیلوه هر کدوم از وز وزن ماهی</t>
   </si>
   <si>
-    <t xml:space="preserve">حالا باید بگیم </t>
+    <t>یه عدد دوتا سینه است تیکه نکردی درسته اره  ا</t>
+  </si>
+  <si>
+    <t xml:space="preserve">حالا باید بگیم ینی ما  الان موخام یارو برا ناهار ساعت یک من هنو دارم سرم گرمه دیدی  مغازم آبروم رفت </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* گوشت چرخ کرده که سفارش داده بودین </t>
+  </si>
+  <si>
+    <t xml:space="preserve">بله جناب ملایی کیا  هستم هردو خروجی چنده </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* فقط آقای بهرامی گفتن که </t>
+  </si>
+  <si>
+    <t>همون درمونگاه ولی عصر  قبلش خب فروشگاه ماس</t>
+  </si>
+  <si>
+    <t>عع یه سوال داشتم از خدمتتون شما گوشت های چرخ کرده تون رو میشوریین یا نه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">عع فراییم زحنت بکشید </t>
   </si>
 </sst>
 </file>
@@ -6146,8 +6164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1843"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6427,7 +6445,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1876</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -6438,6 +6456,9 @@
         <f>HYPERLINK("1739961628_0_SPK_0_20250213_v2.1739437852.2203015.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>1904</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -6448,7 +6469,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -6460,7 +6481,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -6472,7 +6493,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -6484,7 +6505,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -6496,7 +6517,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -6508,16 +6529,19 @@
         <v>Play Audio</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="6" t="str">
+      <c r="B31" s="7" t="str">
         <f>HYPERLINK("1739962354_4_SPK_1_20250216_v2.1739698639.2310716.wav", "Play Audio")</f>
         <v>Play Audio</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>1902</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -6529,7 +6553,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -6541,7 +6565,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -6553,7 +6577,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -6565,7 +6589,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -6577,7 +6601,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -6589,7 +6613,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -6601,7 +6625,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -6613,7 +6637,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -6625,7 +6649,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -6637,7 +6661,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -6661,7 +6685,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1855</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -6673,7 +6697,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -6685,16 +6709,19 @@
         <v>Play Audio</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B46" s="6" t="str">
+      <c r="B46" s="7" t="str">
         <f>HYPERLINK("1739962622_2_SPK_0_20250216_v2.1739720481.2339514.wav", "Play Audio")</f>
         <v>Play Audio</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>1900</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -6706,7 +6733,7 @@
         <v>Play Audio</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -6718,16 +6745,19 @@
         <v>Play Audio</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="6" t="str">
+      <c r="B49" s="7" t="str">
         <f>HYPERLINK("1739962503_0_SPK_1_20250215_v2.1739623381.2279172.wav", "Play Audio")</f>
         <v>Play Audio</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>1901</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -6739,16 +6769,19 @@
         <v>Play Audio</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="6" t="str">
+      <c r="B51" s="7" t="str">
         <f>HYPERLINK("1739961687_4_SPK_0_20250213_v2.1739437852.2203015.wav", "Play Audio")</f>
         <v>Play Audio</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>1897</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -6759,6 +6792,9 @@
         <f>HYPERLINK("1739962432_13_SPK_1_20250215_v2.1739642412.2288835.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C52" s="1" t="s">
+        <v>1855</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
@@ -6768,6 +6804,9 @@
         <f>HYPERLINK("1739962597_15_SPK_0_20250215_v2.1739624662.2279909.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C53" s="1" t="s">
+        <v>1855</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
@@ -6840,6 +6879,9 @@
         <f>HYPERLINK("1739962360_7_SPK_1_20250216_v2.1739716378.2337553.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
+      <c r="C61" s="1" t="s">
+        <v>1855</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
@@ -6868,7 +6910,7 @@
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>66</v>
       </c>
@@ -6877,7 +6919,7 @@
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>67</v>
       </c>
@@ -6886,7 +6928,7 @@
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>68</v>
       </c>
@@ -6894,26 +6936,29 @@
         <f>HYPERLINK("1739962197_4_SPK_0_20250215_v2.1739615161.2265876.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" s="1" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="6" t="str">
+      <c r="B68" s="7" t="str">
         <f>HYPERLINK("1739962519_1_SPK_0_20250217_v2.1739806854.2388719.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="6" t="str">
+      <c r="B69" s="7" t="str">
         <f>HYPERLINK("1739962383_0_SPK_1_20250215_v2.1739615299.2266018.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>71</v>
       </c>
@@ -6922,7 +6967,7 @@
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>72</v>
       </c>
@@ -6930,8 +6975,11 @@
         <f>HYPERLINK("1739963011_7_SPK_0_20250213_v2.1739440064.2207039.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" s="1" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>73</v>
       </c>
@@ -6940,7 +6988,7 @@
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>74</v>
       </c>
@@ -6949,7 +6997,7 @@
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>75</v>
       </c>
@@ -6958,7 +7006,7 @@
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>76</v>
       </c>
@@ -6967,7 +7015,7 @@
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>77</v>
       </c>
@@ -6976,7 +7024,7 @@
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>78</v>
       </c>
@@ -6984,8 +7032,11 @@
         <f>HYPERLINK("1739962691_0_SPK_0_20250218_v2.1739866544.2434478.wav", "Play Audio")</f>
         <v>Play Audio</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77" s="1" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>79</v>
       </c>
@@ -6994,7 +7045,7 @@
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>80</v>
       </c>
@@ -7003,7 +7054,7 @@
         <v>Play Audio</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>81</v>
       </c>

</xml_diff>